<commit_message>
Added new version of the powerpoint for us to display in class
</commit_message>
<xml_diff>
--- a/A1C Info from ADA Publications.xlsx
+++ b/A1C Info from ADA Publications.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Documents/David_Sant/Classes/Systems Modeling BMI 6103/Final Project/systems-modeling-ds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1623937-0488-BC48-83DD-00640E2229C6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2CB8CB-304B-6D40-AA22-A53F247E24BE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="71940" yWindow="3040" windowWidth="27640" windowHeight="16940" xr2:uid="{9F18A06F-BCCD-9348-A81F-0BE70D5CCE9C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19460" activeTab="1" xr2:uid="{9F18A06F-BCCD-9348-A81F-0BE70D5CCE9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,9 @@
     <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
     <sheet name="DMN" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId6"/>
+    <pivotCache cacheId="2" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="423">
   <si>
     <t>HbA1C testing guidelines</t>
   </si>
@@ -1403,12 +1403,6 @@
     <t>56090-4 </t>
   </si>
   <si>
-    <t>67749-2 </t>
-  </si>
-  <si>
-    <t>non-hispanic</t>
-  </si>
-  <si>
     <t>67754-2 </t>
   </si>
   <si>
@@ -1524,13 +1518,19 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tobacco leaf: 852062. </t>
+  </si>
+  <si>
+    <t>Term</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1641,6 +1641,13 @@
       <name val="Times"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1662,7 +1669,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1685,12 +1692,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
@@ -1706,7 +1733,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="7" readingOrder="1"/>
     </xf>
@@ -1723,6 +1749,21 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="7" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3073,7 +3114,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{81CA9B4C-0FD2-B04D-9A04-9DDE033AECD1}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{81CA9B4C-0FD2-B04D-9A04-9DDE033AECD1}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13">
   <location ref="N5:O31" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
@@ -3547,8 +3588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB4B148-0059-4B45-919A-7A7E0EB690FD}">
   <dimension ref="B2:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3700,7 +3741,7 @@
       <c r="D32" s="4"/>
     </row>
     <row r="33" spans="2:5">
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="4"/>
@@ -3790,13 +3831,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2141EFBE-654A-EA47-915E-598040AD2338}">
-  <dimension ref="B2:O54"/>
+  <dimension ref="A2:O55"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="30.5" customWidth="1"/>
+    <col min="3" max="3" width="67" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:2" ht="24">
       <c r="B2" s="6" t="s">
@@ -3838,406 +3886,485 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="2:15" ht="22">
+    <row r="18" spans="1:15" ht="22">
       <c r="B18" s="10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="2:15">
+    <row r="19" spans="1:15">
       <c r="B19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:15">
+    <row r="22" spans="1:15">
       <c r="B22" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="2:15">
+    <row r="23" spans="1:15">
       <c r="B23" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="2:15" ht="24">
+    <row r="26" spans="1:15" ht="24">
       <c r="B26" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="2:15" ht="30">
-      <c r="F28" s="12" t="s">
+    <row r="28" spans="1:15" ht="30">
+      <c r="F28" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="O28" s="14" t="s">
+      <c r="O28" s="13" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="29" spans="2:15">
-      <c r="C29" t="s">
+    <row r="29" spans="1:15" ht="30">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="14"/>
+      <c r="O29" s="13"/>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="14"/>
+      <c r="B30" s="25" t="s">
+        <v>422</v>
+      </c>
+      <c r="C30" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E30" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F30" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G30" s="14"/>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="14"/>
+      <c r="B31" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="26">
+        <v>790.29</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="F31" s="26" t="s">
+        <v>376</v>
+      </c>
+      <c r="G31" s="14"/>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="14"/>
+      <c r="B32" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="26">
+        <v>790.29</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="F32" s="26" t="s">
+        <v>375</v>
+      </c>
+      <c r="G32" s="14"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="14"/>
+      <c r="B33" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="26">
+        <v>790.29</v>
+      </c>
+      <c r="E33" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="F33" s="26" t="s">
+        <v>374</v>
+      </c>
+      <c r="G33" s="14"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="26">
+        <v>250</v>
+      </c>
+      <c r="E34" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F34" s="26" t="s">
+        <v>372</v>
+      </c>
+      <c r="G34" s="14"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="14"/>
+      <c r="B35" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" s="26">
+        <v>250</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F35" s="26" t="s">
+        <v>373</v>
+      </c>
+      <c r="G35" s="14"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="14"/>
+      <c r="B36" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="26">
+        <v>250</v>
+      </c>
+      <c r="E36" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F36" s="26" t="s">
+        <v>372</v>
+      </c>
+      <c r="G36" s="14"/>
+      <c r="I36" s="23" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="14"/>
+      <c r="B37" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" s="26">
+        <v>648.83000000000004</v>
+      </c>
+      <c r="E37" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="F37" s="26"/>
+      <c r="G37" s="14"/>
+      <c r="J37" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="2:15">
-      <c r="B30" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30">
+    <row r="38" spans="1:10">
+      <c r="A38" s="14"/>
+      <c r="B38" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="26">
         <v>790.29</v>
       </c>
-      <c r="E30" t="s">
-        <v>113</v>
-      </c>
-      <c r="F30" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="31" spans="2:15">
-      <c r="B31" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31">
-        <v>790.29</v>
-      </c>
-      <c r="E31" t="s">
-        <v>112</v>
-      </c>
-      <c r="F31" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="32" spans="2:15">
-      <c r="B32" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" t="s">
-        <v>69</v>
-      </c>
-      <c r="D32">
-        <v>790.29</v>
-      </c>
-      <c r="E32" t="s">
-        <v>112</v>
-      </c>
-      <c r="F32" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6">
-      <c r="B33" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" t="s">
-        <v>70</v>
-      </c>
-      <c r="D33">
-        <v>250</v>
-      </c>
-      <c r="E33" t="s">
-        <v>110</v>
-      </c>
-      <c r="F33" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6">
-      <c r="B34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34">
-        <v>250</v>
-      </c>
-      <c r="E34" t="s">
-        <v>111</v>
-      </c>
-      <c r="F34" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6">
-      <c r="B35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" t="s">
-        <v>75</v>
-      </c>
-      <c r="D35">
-        <v>250</v>
-      </c>
-      <c r="E35" t="s">
-        <v>110</v>
-      </c>
-      <c r="F35" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6">
-      <c r="B36" t="s">
-        <v>73</v>
-      </c>
-      <c r="C36" t="s">
-        <v>76</v>
-      </c>
-      <c r="D36">
-        <v>648.83000000000004</v>
-      </c>
-      <c r="E36" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6">
-      <c r="B37" t="s">
-        <v>58</v>
-      </c>
-      <c r="C37" t="s">
-        <v>77</v>
-      </c>
-      <c r="D37">
-        <v>790.29</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="E38" s="26" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="38" spans="2:6">
-      <c r="B38" t="s">
+      <c r="F38" s="26"/>
+      <c r="G38" s="14"/>
+      <c r="I38" t="s">
+        <v>421</v>
+      </c>
+      <c r="J38">
+        <v>852062</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="14"/>
+      <c r="B39" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D38">
+      <c r="D39" s="26">
         <v>278</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E39" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F39" s="26" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="39" spans="2:6">
-      <c r="B39" t="s">
+      <c r="G39" s="14"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="14"/>
+      <c r="B40" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="F39" t="s">
+      <c r="E40" s="26"/>
+      <c r="F40" s="26" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="40" spans="2:6">
-      <c r="B40" t="s">
+      <c r="G40" s="14"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="14"/>
+      <c r="B41" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="F40" t="s">
+      <c r="E41" s="26"/>
+      <c r="F41" s="26" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="41" spans="2:6">
-      <c r="B41" t="s">
+      <c r="G41" s="14"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="14"/>
+      <c r="B42" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="F41" t="s">
+      <c r="E42" s="26"/>
+      <c r="F42" s="26" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="42" spans="2:6">
-      <c r="B42" t="s">
+      <c r="G42" s="14"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="14"/>
+      <c r="B43" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="D42" t="s">
+      <c r="C43" s="14"/>
+      <c r="D43" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="F42" t="s">
+      <c r="E43" s="26"/>
+      <c r="F43" s="26" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="43" spans="2:6">
-      <c r="B43" t="s">
+      <c r="G43" s="14"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="14"/>
+      <c r="B44" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="F43" t="s">
+      <c r="E44" s="26"/>
+      <c r="F44" s="26" t="s">
+        <v>382</v>
+      </c>
+      <c r="G44" s="14"/>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="14"/>
+      <c r="B45" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="G45" s="14"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="14"/>
+      <c r="B46" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="E46" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="F46" s="26" t="s">
+        <v>383</v>
+      </c>
+      <c r="G46" s="14"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="14"/>
+      <c r="B47" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D47" s="26">
+        <v>401.9</v>
+      </c>
+      <c r="E47" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="F47" s="26" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="44" spans="2:6">
-      <c r="B44" t="s">
-        <v>94</v>
-      </c>
-      <c r="C44" t="s">
-        <v>92</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="G47" s="14"/>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="14"/>
+      <c r="B48" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D48" s="26">
+        <v>272</v>
+      </c>
+      <c r="E48" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="F48" s="26" t="s">
+        <v>385</v>
+      </c>
+      <c r="G48" s="14"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="14"/>
+      <c r="B49" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D49" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="F44" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6">
-      <c r="B45" t="s">
-        <v>60</v>
-      </c>
-      <c r="C45" t="s">
-        <v>78</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="E49" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="F49" s="26" t="s">
+        <v>386</v>
+      </c>
+      <c r="G49" s="14"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="14"/>
+      <c r="B50" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D50" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="E45" t="s">
-        <v>99</v>
-      </c>
-      <c r="F45" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6">
-      <c r="B46" t="s">
-        <v>61</v>
-      </c>
-      <c r="C46" t="s">
-        <v>79</v>
-      </c>
-      <c r="D46">
-        <v>401.9</v>
-      </c>
-      <c r="E46" t="s">
-        <v>106</v>
-      </c>
-      <c r="F46" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6">
-      <c r="B47" t="s">
-        <v>80</v>
-      </c>
-      <c r="C47" t="s">
-        <v>81</v>
-      </c>
-      <c r="D47">
-        <v>272</v>
-      </c>
-      <c r="E47" t="s">
-        <v>105</v>
-      </c>
-      <c r="F47" t="s">
+      <c r="E50" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="F50" s="26" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="48" spans="2:6">
-      <c r="B48" t="s">
-        <v>82</v>
-      </c>
-      <c r="C48" t="s">
-        <v>83</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="G50" s="14"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="14"/>
+      <c r="B51" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D51" s="26">
+        <v>256.39999999999998</v>
+      </c>
+      <c r="E51" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="F51" s="26"/>
+      <c r="G51" s="14"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="14"/>
+      <c r="B52" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="D52" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="E48" t="s">
-        <v>102</v>
-      </c>
-      <c r="F48" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8">
-      <c r="B49" t="s">
-        <v>26</v>
-      </c>
-      <c r="C49" t="s">
-        <v>95</v>
-      </c>
-      <c r="D49" t="s">
-        <v>100</v>
-      </c>
-      <c r="E49" t="s">
-        <v>103</v>
-      </c>
-      <c r="F49" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8">
-      <c r="B50" t="s">
-        <v>62</v>
-      </c>
-      <c r="C50" t="s">
-        <v>97</v>
-      </c>
-      <c r="D50">
-        <v>256.39999999999998</v>
-      </c>
-      <c r="E50" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8">
-      <c r="B51" t="s">
-        <v>63</v>
-      </c>
-      <c r="C51" t="s">
-        <v>96</v>
-      </c>
-      <c r="D51" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" ht="20">
-      <c r="B52" s="11"/>
-    </row>
-    <row r="53" spans="2:8">
-      <c r="H53" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" ht="31">
-      <c r="H54" s="17" t="s">
-        <v>382</v>
-      </c>
+      <c r="E52" s="28"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="14"/>
+    </row>
+    <row r="53" spans="1:8" ht="20">
+      <c r="A53" s="14"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+    </row>
+    <row r="55" spans="1:8" ht="31">
+      <c r="H55" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4248,7 +4375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{336966E2-5E89-CE4C-8E45-1029EBE4E177}">
   <dimension ref="A1:O250"/>
   <sheetViews>
-    <sheetView topLeftCell="B21" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="B11" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
@@ -4262,250 +4389,250 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15" t="s">
         <v>369</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>371</v>
       </c>
-      <c r="E2" s="15"/>
+      <c r="E2" s="14"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16">
+      <c r="A3" s="14"/>
+      <c r="B3" s="15">
         <v>1</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="15">
         <v>30.5</v>
       </c>
-      <c r="E3" s="15"/>
+      <c r="E3" s="14"/>
       <c r="F3" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16">
+      <c r="A4" s="14"/>
+      <c r="B4" s="15">
         <v>2</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="15">
         <v>27.3</v>
       </c>
-      <c r="E4" s="15"/>
+      <c r="E4" s="14"/>
       <c r="F4" s="2" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16">
+      <c r="A5" s="14"/>
+      <c r="B5" s="15">
         <v>3</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="15">
         <v>24.1</v>
       </c>
-      <c r="E5" s="15"/>
+      <c r="E5" s="14"/>
       <c r="F5" t="s">
         <v>367</v>
       </c>
-      <c r="N5" s="18" t="s">
+      <c r="N5" s="17" t="s">
+        <v>388</v>
+      </c>
+      <c r="O5" t="s">
         <v>390</v>
       </c>
-      <c r="O5" t="s">
-        <v>392</v>
-      </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15">
         <v>4</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="15">
         <v>23.4</v>
       </c>
-      <c r="E6" s="15"/>
+      <c r="E6" s="14"/>
       <c r="F6" t="s">
         <v>368</v>
       </c>
-      <c r="N6" s="19" t="s">
+      <c r="N6" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="O6" s="20">
+      <c r="O6" s="19">
         <v>30.5</v>
       </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15">
         <v>5</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="15">
         <v>22.7</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="N7" s="19" t="s">
+      <c r="E7" s="14"/>
+      <c r="N7" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="O7" s="20">
+      <c r="O7" s="19">
         <v>27.3</v>
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15">
         <v>6</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="15">
         <v>22.6</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="N8" s="19" t="s">
+      <c r="E8" s="14"/>
+      <c r="N8" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="O8" s="20">
+      <c r="O8" s="19">
         <v>24.1</v>
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15">
         <v>7</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="15">
         <v>22</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="N9" s="19" t="s">
+      <c r="E9" s="14"/>
+      <c r="N9" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="O9" s="20">
+      <c r="O9" s="19">
         <v>23.4</v>
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15">
         <v>8</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="15">
         <v>21.5</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="N10" s="19" t="s">
+      <c r="E10" s="14"/>
+      <c r="N10" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="O10" s="20">
+      <c r="O10" s="19">
         <v>22.7</v>
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16">
+      <c r="A11" s="14"/>
+      <c r="B11" s="15">
         <v>9</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="15">
         <v>18.7</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="N11" s="19" t="s">
+      <c r="E11" s="14"/>
+      <c r="N11" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="O11" s="20">
+      <c r="O11" s="19">
         <v>22.6</v>
       </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15">
         <v>10</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="15">
         <v>17.7</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="N12" s="19" t="s">
+      <c r="E12" s="14"/>
+      <c r="N12" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="O12" s="20">
+      <c r="O12" s="19">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14">
         <v>11</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="14">
         <v>17.600000000000001</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="N13" s="19" t="s">
+      <c r="E13" s="14"/>
+      <c r="N13" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="O13" s="20">
+      <c r="O13" s="19">
         <v>21.5</v>
       </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14">
         <v>12</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="14">
         <v>17.3</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="N14" s="19" t="s">
+      <c r="E14" s="14"/>
+      <c r="N14" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="O14" s="20">
+      <c r="O14" s="19">
         <v>18.7</v>
       </c>
     </row>
@@ -4519,10 +4646,10 @@
       <c r="D15">
         <v>17.3</v>
       </c>
-      <c r="N15" s="19" t="s">
+      <c r="N15" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="O15" s="20">
+      <c r="O15" s="19">
         <v>17.7</v>
       </c>
     </row>
@@ -4536,10 +4663,10 @@
       <c r="D16">
         <v>17.100000000000001</v>
       </c>
-      <c r="N16" s="19" t="s">
+      <c r="N16" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="O16" s="20">
+      <c r="O16" s="19">
         <v>17.600000000000001</v>
       </c>
     </row>
@@ -4553,10 +4680,10 @@
       <c r="D17">
         <v>16.7</v>
       </c>
-      <c r="N17" s="19" t="s">
+      <c r="N17" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="O17" s="20">
+      <c r="O17" s="19">
         <v>17.3</v>
       </c>
     </row>
@@ -4570,10 +4697,10 @@
       <c r="D18">
         <v>16.5</v>
       </c>
-      <c r="N18" s="19" t="s">
+      <c r="N18" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="O18" s="20">
+      <c r="O18" s="19">
         <v>17.3</v>
       </c>
     </row>
@@ -4587,10 +4714,10 @@
       <c r="D19">
         <v>16.5</v>
       </c>
-      <c r="N19" s="19" t="s">
+      <c r="N19" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="O19" s="20">
+      <c r="O19" s="19">
         <v>17.100000000000001</v>
       </c>
     </row>
@@ -4604,10 +4731,10 @@
       <c r="D20">
         <v>15.9</v>
       </c>
-      <c r="N20" s="19" t="s">
+      <c r="N20" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="O20" s="20">
+      <c r="O20" s="19">
         <v>16.7</v>
       </c>
     </row>
@@ -4621,10 +4748,10 @@
       <c r="D21">
         <v>15.8</v>
       </c>
-      <c r="N21" s="19" t="s">
+      <c r="N21" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="O21" s="20">
+      <c r="O21" s="19">
         <v>16.5</v>
       </c>
     </row>
@@ -4638,10 +4765,10 @@
       <c r="D22">
         <v>15.7</v>
       </c>
-      <c r="N22" s="19" t="s">
+      <c r="N22" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="O22" s="20">
+      <c r="O22" s="19">
         <v>16.5</v>
       </c>
     </row>
@@ -4655,10 +4782,10 @@
       <c r="D23">
         <v>15.4</v>
       </c>
-      <c r="N23" s="19" t="s">
+      <c r="N23" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="O23" s="20">
+      <c r="O23" s="19">
         <v>15.9</v>
       </c>
     </row>
@@ -4672,10 +4799,10 @@
       <c r="D24">
         <v>14.5</v>
       </c>
-      <c r="N24" s="19" t="s">
+      <c r="N24" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="O24" s="20">
+      <c r="O24" s="19">
         <v>15.8</v>
       </c>
     </row>
@@ -4689,10 +4816,10 @@
       <c r="D25">
         <v>13.7</v>
       </c>
-      <c r="N25" s="19" t="s">
+      <c r="N25" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="O25" s="20">
+      <c r="O25" s="19">
         <v>15.7</v>
       </c>
     </row>
@@ -4706,10 +4833,10 @@
       <c r="D26">
         <v>13.6</v>
       </c>
-      <c r="N26" s="19" t="s">
+      <c r="N26" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="O26" s="20">
+      <c r="O26" s="19">
         <v>15.4</v>
       </c>
     </row>
@@ -4723,10 +4850,10 @@
       <c r="D27">
         <v>13.2</v>
       </c>
-      <c r="N27" s="19" t="s">
+      <c r="N27" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="O27" s="20">
+      <c r="O27" s="19">
         <v>14.5</v>
       </c>
     </row>
@@ -4740,10 +4867,10 @@
       <c r="D28">
         <v>13.2</v>
       </c>
-      <c r="N28" s="19" t="s">
+      <c r="N28" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="O28" s="20">
+      <c r="O28" s="19">
         <v>13.7</v>
       </c>
     </row>
@@ -4757,10 +4884,10 @@
       <c r="D29">
         <v>13.2</v>
       </c>
-      <c r="N29" s="19" t="s">
+      <c r="N29" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="O29" s="20">
+      <c r="O29" s="19">
         <v>13.6</v>
       </c>
     </row>
@@ -4774,10 +4901,10 @@
       <c r="D30">
         <v>13.1</v>
       </c>
-      <c r="N30" s="19" t="s">
+      <c r="N30" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="O30" s="20">
+      <c r="O30" s="19">
         <v>13.2</v>
       </c>
     </row>
@@ -4791,10 +4918,10 @@
       <c r="D31">
         <v>13</v>
       </c>
-      <c r="N31" s="19" t="s">
-        <v>391</v>
-      </c>
-      <c r="O31" s="20">
+      <c r="N31" s="18" t="s">
+        <v>389</v>
+      </c>
+      <c r="O31" s="19">
         <v>467.29999999999995</v>
       </c>
     </row>
@@ -5041,13 +5168,13 @@
       </c>
     </row>
     <row r="54" spans="2:4">
-      <c r="B54" s="13">
+      <c r="B54" s="12">
         <v>52</v>
       </c>
-      <c r="C54" s="13" t="s">
+      <c r="C54" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="D54" s="13">
+      <c r="D54" s="12">
         <v>10.8</v>
       </c>
     </row>
@@ -7078,23 +7205,23 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D1" t="s">
         <v>393</v>
-      </c>
-      <c r="C1" t="s">
-        <v>394</v>
-      </c>
-      <c r="D1" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B3">
         <v>7.82</v>
@@ -7122,384 +7249,384 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22" t="s">
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21" t="s">
+        <v>396</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>398</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21" t="s">
+        <v>404</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21" t="s">
+        <v>397</v>
+      </c>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21" t="s">
+        <v>396</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21" t="s">
+        <v>399</v>
+      </c>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21" t="s">
+        <v>396</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21" t="s">
         <v>400</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22" t="s">
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21" t="s">
+        <v>396</v>
+      </c>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21" t="s">
+        <v>396</v>
+      </c>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21" t="s">
+        <v>396</v>
+      </c>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="22" t="s">
+        <v>401</v>
+      </c>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21" t="s">
+        <v>396</v>
+      </c>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22" t="s">
+        <v>402</v>
+      </c>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21" t="s">
+        <v>396</v>
+      </c>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22" t="s">
+        <v>403</v>
+      </c>
+      <c r="M9" s="22"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21" t="s">
+        <v>396</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="21" t="s">
+        <v>405</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21" t="s">
         <v>406</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22" t="s">
-        <v>399</v>
-      </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22" t="s">
-        <v>398</v>
-      </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22" t="s">
-        <v>401</v>
-      </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22" t="s">
-        <v>398</v>
-      </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22" t="s">
-        <v>402</v>
-      </c>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22" t="s">
-        <v>398</v>
-      </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22" t="s">
-        <v>398</v>
-      </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22" t="s">
-        <v>398</v>
-      </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="23" t="s">
-        <v>403</v>
-      </c>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22" t="s">
-        <v>398</v>
-      </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23" t="s">
-        <v>404</v>
-      </c>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="22"/>
-    </row>
-    <row r="9" spans="1:17">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22" t="s">
-        <v>398</v>
-      </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23" t="s">
-        <v>405</v>
-      </c>
-      <c r="M9" s="23"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22" t="s">
-        <v>398</v>
-      </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="A11" s="22" t="s">
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21" t="s">
         <v>407</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="22"/>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22" t="s">
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21" t="s">
         <v>408</v>
       </c>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="22"/>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22" t="s">
-        <v>409</v>
-      </c>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="22"/>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22" t="s">
-        <v>410</v>
-      </c>
-      <c r="Q14" s="22"/>
+      <c r="Q14" s="21"/>
     </row>
     <row r="15" spans="1:17">
       <c r="B15" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="B16" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>